<commit_message>
Update Bill of Material quantum dice.xlsx
</commit_message>
<xml_diff>
--- a/3D print files/Bill of Material quantum dice.xlsx
+++ b/3D print files/Bill of Material quantum dice.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aernoutvanrossum/Github/quantumdice-by-utwente/3D print files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aernoutvanrossum/Github/QD-prod/Quantum-Dice-by-UTwente/3D print files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5342625D-4C35-944E-B765-AB80725753C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CF6B17-4916-DB46-A234-31B17EE1BBB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{281531AD-289F-7444-9810-C417D6306E6A}"/>
   </bookViews>
@@ -267,7 +267,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="79">
   <si>
     <t>1.28 inch IPS Color TFT LCD Display Module 1.28" RGB LED Round Touch Screen GC9A01 Drive 4 Wire SPI Interface 240x240 PCB Board</t>
   </si>
@@ -489,6 +489,21 @@
   </si>
   <si>
     <t>https://gitlab.utwente.nl/m7695371/quantumdice-by-utwente/-/tree/main/3D%20print%20files/quantum%20dice%203D%20print%20parts%20TPUFrameOnly?ref_type=heads</t>
+  </si>
+  <si>
+    <t>blue PLA</t>
+  </si>
+  <si>
+    <t>red PLA</t>
+  </si>
+  <si>
+    <t>yellow PLA</t>
+  </si>
+  <si>
+    <t>TPU</t>
+  </si>
+  <si>
+    <t>3D print material masses (gram)</t>
   </si>
 </sst>
 </file>
@@ -498,7 +513,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;€&quot;\ * #,##0.00_);_(&quot;€&quot;\ * \(#,##0.00\);_(&quot;€&quot;\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -548,6 +563,12 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -571,7 +592,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -580,6 +601,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -597,10 +619,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -920,10 +938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B6AF03-25E8-2042-B8EE-7BB1F35ABDC9}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1532,6 +1550,80 @@
     <row r="48" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B48" s="3" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B50" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51">
+        <f t="shared" ref="C51:C54" si="2">$C$2*D51+$C$3*E51</f>
+        <v>55</v>
+      </c>
+      <c r="D51" s="4">
+        <f>55/2</f>
+        <v>27.5</v>
+      </c>
+      <c r="E51" s="4">
+        <f>55/2</f>
+        <v>27.5</v>
+      </c>
+      <c r="F51" s="8"/>
+    </row>
+    <row r="52" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>75</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="D52" s="4">
+        <f>58/2</f>
+        <v>29</v>
+      </c>
+      <c r="E52" s="4">
+        <f>58/2</f>
+        <v>29</v>
+      </c>
+      <c r="F52" s="8"/>
+    </row>
+    <row r="53" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>76</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="2"/>
+        <v>66</v>
+      </c>
+      <c r="D53" s="4">
+        <v>33</v>
+      </c>
+      <c r="E53" s="4">
+        <v>33</v>
+      </c>
+      <c r="F53" s="8"/>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>77</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="2"/>
+        <v>126</v>
+      </c>
+      <c r="D54" s="4">
+        <f>126/2</f>
+        <v>63</v>
+      </c>
+      <c r="E54" s="4">
+        <f>126/2</f>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1658,7 +1750,7 @@
         <v>7</v>
       </c>
       <c r="C12">
-        <f t="shared" ref="C12:C39" si="0">$C$2*D12+$C$3*E12</f>
+        <f t="shared" ref="C12:C28" si="0">$C$2*D12+$C$3*E12</f>
         <v>2</v>
       </c>
       <c r="D12" s="4">
@@ -1930,7 +2022,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <f t="shared" ref="C31:C47" si="1">$C$2*D31+$C$3*E31</f>
+        <f t="shared" ref="C31:C35" si="1">$C$2*D31+$C$3*E31</f>
         <v>12</v>
       </c>
       <c r="D31" s="4">
@@ -2179,15 +2271,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="5f810545-bb7d-498e-98a6-3cc8175571c8">
@@ -2196,6 +2279,15 @@
     <TaxCatchAll xmlns="8077f6fe-c9e5-4688-b004-da2992bb8cd8" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2406,14 +2498,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA44028-4133-420E-8665-60C989F4E89B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D196A880-6C6D-4D69-8998-929C3B39CF40}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -2426,6 +2510,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="8077f6fe-c9e5-4688-b004-da2992bb8cd8"/>
     <ds:schemaRef ds:uri="5f810545-bb7d-498e-98a6-3cc8175571c8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA44028-4133-420E-8665-60C989F4E89B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added 3D printmaterial masses; updated links
</commit_message>
<xml_diff>
--- a/3D print files/Bill of Material quantum dice.xlsx
+++ b/3D print files/Bill of Material quantum dice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aernoutvanrossum/Github/QD-prod/Quantum-Dice-by-UTwente/3D print files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CF6B17-4916-DB46-A234-31B17EE1BBB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B4CE8E-EA42-2541-AFD2-97871331CD68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{281531AD-289F-7444-9810-C417D6306E6A}"/>
   </bookViews>
@@ -42,6 +42,39 @@
     <author>Aernout van Rossum</author>
   </authors>
   <commentList>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{DFB0096F-A5DB-A649-BD54-16CED2FE5E40}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">A set of Quantum Dices requires a Role A and a Role B </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fill in the #Role A and #Role B</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B3" authorId="0" shapeId="0" xr:uid="{B126064D-5697-EE42-A154-2E468E42DB06}">
       <text>
         <r>
@@ -157,6 +190,30 @@
     <author>Aernout van Rossum</author>
   </authors>
   <commentList>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{CFE3BC6F-2491-DF42-AE84-26631EFB2E53}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">A set of Quantum Dices requires a Role A and a Role B 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Fill in the #Role A and #Role B
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B3" authorId="0" shapeId="0" xr:uid="{C9F00DD2-6E01-F84C-8803-820683ECAF24}">
       <text>
         <r>
@@ -267,7 +324,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="85">
   <si>
     <t>1.28 inch IPS Color TFT LCD Display Module 1.28" RGB LED Round Touch Screen GC9A01 Drive 4 Wire SPI Interface 240x240 PCB Board</t>
   </si>
@@ -485,12 +542,6 @@
     <t>frame parts and cups all TPU</t>
   </si>
   <si>
-    <t>https://gitlab.utwente.nl/m7695371/quantumdice-by-utwente/-/tree/main/3D%20print%20files/quantum%20dice%203D%20print%20parts%20AllTPU?ref_type=heads</t>
-  </si>
-  <si>
-    <t>https://gitlab.utwente.nl/m7695371/quantumdice-by-utwente/-/tree/main/3D%20print%20files/quantum%20dice%203D%20print%20parts%20TPUFrameOnly?ref_type=heads</t>
-  </si>
-  <si>
     <t>blue PLA</t>
   </si>
   <si>
@@ -503,7 +554,31 @@
     <t>TPU</t>
   </si>
   <si>
-    <t>3D print material masses (gram)</t>
+    <t>https://github.com/qlab-utwente/Quantum-Dice-by-UTwente/tree/main/3D%20print%20files/quantum%20dice%203D%20print%20parts%20TPUFrameOnly</t>
+  </si>
+  <si>
+    <t>https://github.com/qlab-utwente/Quantum-Dice-by-UTwente/tree/main/3D%20print%20files/quantum%20dice%203D%20print%20parts%20AllTPU</t>
+  </si>
+  <si>
+    <t>blue TPU</t>
+  </si>
+  <si>
+    <t>red TPU</t>
+  </si>
+  <si>
+    <t>yellow TPU</t>
+  </si>
+  <si>
+    <t>frame TPU</t>
+  </si>
+  <si>
+    <t>backplanes white PLA</t>
+  </si>
+  <si>
+    <t>tbd</t>
+  </si>
+  <si>
+    <t>Estimated 3D print material masses (gram)</t>
   </si>
 </sst>
 </file>
@@ -619,6 +694,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -941,7 +1020,7 @@
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1029,7 +1108,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1047,7 +1126,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1065,7 +1144,7 @@
         <v>2</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1083,7 +1162,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1101,7 +1180,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1119,7 +1198,7 @@
         <v>2</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
@@ -1137,7 +1216,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
@@ -1153,7 +1232,7 @@
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
@@ -1168,7 +1247,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
@@ -1186,7 +1265,7 @@
         <v>4</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
@@ -1204,7 +1283,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
@@ -1222,7 +1301,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
@@ -1554,12 +1633,12 @@
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B50" s="2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" spans="2:6" ht="17" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C51">
         <f t="shared" ref="C51:C54" si="2">$C$2*D51+$C$3*E51</f>
@@ -1577,7 +1656,7 @@
     </row>
     <row r="52" spans="2:6" ht="17" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C52">
         <f t="shared" si="2"/>
@@ -1595,7 +1674,7 @@
     </row>
     <row r="53" spans="2:6" ht="17" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C53">
         <f t="shared" si="2"/>
@@ -1611,7 +1690,7 @@
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C54">
         <f t="shared" si="2"/>
@@ -1641,8 +1720,8 @@
     <hyperlink ref="F39" r:id="rId11" xr:uid="{4CA5F8F4-9815-8942-B98E-8375FCA3C7B2}"/>
     <hyperlink ref="F40" r:id="rId12" xr:uid="{9DC6EDF5-311E-084A-AD02-E0859B9D1D78}"/>
     <hyperlink ref="F35" r:id="rId13" xr:uid="{4D119E3A-09A7-884C-B9FF-09D40E8F4386}"/>
-    <hyperlink ref="F11" r:id="rId14" xr:uid="{929151B0-CF35-8948-9351-D57C1913FD54}"/>
-    <hyperlink ref="F12:F22" r:id="rId15" display="https://gitlab.utwente.nl/m7695371/quantumdice-by-utwente/-/tree/main/3D%20print%20files/quantum%20dice%203D%20print%20parts%20TPUFrameOnly?ref_type=heads" xr:uid="{D2149FA7-34B8-AB46-8CED-3CE88B2BA9B1}"/>
+    <hyperlink ref="F11" r:id="rId14" xr:uid="{69EE7F58-86AB-5C42-9D90-993C46E8D321}"/>
+    <hyperlink ref="F12:F22" r:id="rId15" display="https://github.com/qlab-utwente/Quantum-Dice-by-UTwente/tree/main/3D%20print%20files/quantum%20dice%203D%20print%20parts%20TPUFrameOnly" xr:uid="{F1AB62F5-AC28-0A43-9BB4-0725CAEB4FF4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId16"/>
@@ -1651,10 +1730,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC5DF7A8-08FA-2145-BADA-18AB879783DA}">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1742,7 +1821,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1760,7 +1839,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1778,7 +1857,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1796,7 +1875,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1814,7 +1893,7 @@
         <v>2</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1832,7 +1911,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
@@ -1848,7 +1927,7 @@
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
@@ -1863,7 +1942,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
@@ -1881,7 +1960,7 @@
         <v>4</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
@@ -1899,7 +1978,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
@@ -1917,7 +1996,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
@@ -2245,6 +2324,68 @@
     <row r="47" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B47" s="3" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B50" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>78</v>
+      </c>
+      <c r="C51">
+        <f t="shared" ref="C51:C54" si="3">$C$2*D51+$C$3*E51</f>
+        <v>0</v>
+      </c>
+      <c r="E51" s="4"/>
+      <c r="F51" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>79</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E52" s="4"/>
+      <c r="F52" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>80</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E53" s="4"/>
+      <c r="F53" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>81</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E54" s="4"/>
+      <c r="F54" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2262,35 +2403,13 @@
     <hyperlink ref="F38" r:id="rId11" xr:uid="{B59C96D6-FB81-F446-BB1B-1BFFEE168540}"/>
     <hyperlink ref="F39" r:id="rId12" xr:uid="{DC25E6C6-FB14-0A43-B2F2-7DEDB09B8DE5}"/>
     <hyperlink ref="F34" r:id="rId13" xr:uid="{7AC34CA2-FD87-3141-90BF-E0149B164C1E}"/>
-    <hyperlink ref="F11" r:id="rId14" xr:uid="{06D6FA9B-EC5A-FD40-BE50-E48635E12AFB}"/>
-    <hyperlink ref="F12:F21" r:id="rId15" display="https://gitlab.utwente.nl/m7695371/quantumdice-by-utwente/-/tree/main/3D%20print%20files/quantum%20dice%203D%20print%20parts%20AllTPU?ref_type=heads" xr:uid="{8B25FFC2-5745-2F48-9869-865CB1D9FE99}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId16"/>
+  <legacyDrawing r:id="rId14"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5f810545-bb7d-498e-98a6-3cc8175571c8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="8077f6fe-c9e5-4688-b004-da2992bb8cd8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FF458063C0B8354687E7E385217DADDD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="db0b04aaa15c7297f6f6526469376690">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5f810545-bb7d-498e-98a6-3cc8175571c8" xmlns:ns3="8077f6fe-c9e5-4688-b004-da2992bb8cd8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="66dfeb35f9f6b101ff511922eb62fa51" ns2:_="" ns3:_="">
     <xsd:import namespace="5f810545-bb7d-498e-98a6-3cc8175571c8"/>
@@ -2497,32 +2616,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D196A880-6C6D-4D69-8998-929C3B39CF40}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="8077f6fe-c9e5-4688-b004-da2992bb8cd8"/>
-    <ds:schemaRef ds:uri="5f810545-bb7d-498e-98a6-3cc8175571c8"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA44028-4133-420E-8665-60C989F4E89B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5f810545-bb7d-498e-98a6-3cc8175571c8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="8077f6fe-c9e5-4688-b004-da2992bb8cd8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC96DF67-5917-4890-8162-737ED9540272}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2539,4 +2653,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA44028-4133-420E-8665-60C989F4E89B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D196A880-6C6D-4D69-8998-929C3B39CF40}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="8077f6fe-c9e5-4688-b004-da2992bb8cd8"/>
+    <ds:schemaRef ds:uri="5f810545-bb7d-498e-98a6-3cc8175571c8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update Bill of Material for quantum dice
Revised the Bill of Material spreadsheet for the quantum dice project. Changes may include updated components, quantities, or specifications.
</commit_message>
<xml_diff>
--- a/3D print files/Bill of Material quantum dice.xlsx
+++ b/3D print files/Bill of Material quantum dice.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aernoutvanrossum/Github/Quantum-Dice-by-UTwente/3D print files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A81BAD5-8F7C-264E-87D7-BDB156038A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AD8110-FC91-554F-BD39-36809DF21B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7760" yWindow="860" windowWidth="28800" windowHeight="15800" xr2:uid="{281531AD-289F-7444-9810-C417D6306E6A}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="28800" windowHeight="15800" xr2:uid="{281531AD-289F-7444-9810-C417D6306E6A}"/>
   </bookViews>
   <sheets>
     <sheet name="TPUFrameOnly" sheetId="2" r:id="rId1"/>
@@ -261,103 +261,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="B31" authorId="0" shapeId="0" xr:uid="{C53E167F-8051-B048-BC6C-FF5B30EF71FC}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">In rare situations the display module is Dead On Arrival (DOA). Order some extra display units
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B34" authorId="0" shapeId="0" xr:uid="{32530371-7491-5143-B4E3-59E2B0404689}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Content of cable set see below</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B35" authorId="0" shapeId="0" xr:uid="{878487E2-8FD2-0F4B-B286-91D511B9A2E5}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>3.7V lipo battery:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Size: maximum 50mm high/width. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Thickness: max 15 mm
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Capacitiy: 1000 - 1500 mAh. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Connector: JST plug (red) or JST-PH (2 pole), 2mm
-</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="85">
   <si>
     <t>1.28 inch IPS Color TFT LCD Display Module 1.28" RGB LED Round Touch Screen GC9A01 Drive 4 Wire SPI Interface 240x240 PCB Board</t>
   </si>
@@ -419,9 +328,6 @@
     <t>Allen countersunk head screw, M3x6</t>
   </si>
   <si>
-    <t>Allen cylinder head screw, M3x20</t>
-  </si>
-  <si>
     <t>Whislist</t>
   </si>
   <si>
@@ -434,9 +340,6 @@
     <t>https://www.fabory.com/nl/cilinderschroef-met-binnenzeskant-din-912-roestvaststaal-%28rvs%29-a2-m3x6/p/51050030006</t>
   </si>
   <si>
-    <t>https://www.fabory.com/nl/cilinderschroef-met-binnenzeskant-din-912-roestvaststaal-%28rvs%29-a2-m3x20/p/51050030020</t>
-  </si>
-  <si>
     <t>https://www.fabory.com/nl/verzonken-schroef-met-binnenzeskant-iso-10642-staal-blank-010-9-m3x6/p/07400030006</t>
   </si>
   <si>
@@ -473,18 +376,12 @@
     <t>USB charge cable with USB-C Connector Type-C to PH 2.0 black</t>
   </si>
   <si>
-    <t>https://eu.robotshop.com/nl/products/bricogeek-lipo-batterij-37v-1100mah-20c-geschikt-voor-rc-en-drones?qd=7948839c00036b1858e2c8d27aac19e8</t>
-  </si>
-  <si>
     <t>Number of dice</t>
   </si>
   <si>
     <t>dice type</t>
   </si>
   <si>
-    <t>Lipo-batterij 3.7V, 1100mAh 20C1100mAh, model 903048</t>
-  </si>
-  <si>
     <t>03A_White_PLA_V*_display_mount</t>
   </si>
   <si>
@@ -563,9 +460,6 @@
     <t>Optional NOT NEEDED when a complete set is ordered @Utwnte</t>
   </si>
   <si>
-    <t>Optional NOT NEEDED when a complete set is ordered @Utwente</t>
-  </si>
-  <si>
     <t>Quantum Dice Role A TPUFrameOnly</t>
   </si>
   <si>
@@ -624,6 +518,9 @@
   </si>
   <si>
     <t>https://www.aliexpress.us/item/3256809160966846.html?gatewayAdapt=glo2usa4itemAdapt</t>
+  </si>
+  <si>
+    <t>see tab "TPUFrameOnly"</t>
   </si>
 </sst>
 </file>
@@ -1060,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B6AF03-25E8-2042-B8EE-7BB1F35ABDC9}">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1076,45 +973,45 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="7"/>
       <c r="F1" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1131,7 +1028,7 @@
         <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1149,7 +1046,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1167,12 +1064,12 @@
         <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
@@ -1185,12 +1082,12 @@
         <v>2</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
@@ -1203,7 +1100,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1221,7 +1118,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1239,7 +1136,7 @@
         <v>2</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
@@ -1257,7 +1154,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
@@ -1273,7 +1170,7 @@
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
@@ -1288,12 +1185,12 @@
         <v>1</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
@@ -1306,12 +1203,12 @@
         <v>4</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
@@ -1324,12 +1221,12 @@
         <v>1</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
@@ -1342,7 +1239,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
@@ -1365,7 +1262,7 @@
         <v>6</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
@@ -1383,12 +1280,12 @@
         <v>24</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
@@ -1401,12 +1298,12 @@
         <v>12</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C28">
         <f t="shared" si="0"/>
@@ -1421,7 +1318,7 @@
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C29">
         <f t="shared" si="0"/>
@@ -1434,7 +1331,7 @@
         <v>4</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.2">
@@ -1457,12 +1354,12 @@
         <v>6</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C33">
         <f t="shared" si="0"/>
@@ -1475,12 +1372,12 @@
         <v>1</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C34">
         <f t="shared" si="0"/>
@@ -1493,12 +1390,12 @@
         <v>1</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C35">
         <f t="shared" si="0"/>
@@ -1511,12 +1408,12 @@
         <v>1</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C36">
         <f t="shared" si="0"/>
@@ -1529,7 +1426,7 @@
         <v>1</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.2">
@@ -1537,15 +1434,15 @@
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F38" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C39">
         <f t="shared" ref="C39:C44" si="1">$C$2*D39+$C$3*E39</f>
@@ -1563,7 +1460,7 @@
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C40">
         <f t="shared" si="1"/>
@@ -1576,12 +1473,12 @@
         <v>1</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C41">
         <f t="shared" si="1"/>
@@ -1594,12 +1491,12 @@
         <v>1</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C42">
         <f t="shared" si="1"/>
@@ -1612,12 +1509,12 @@
         <v>1</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C43">
         <f t="shared" si="1"/>
@@ -1630,12 +1527,12 @@
         <v>4</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C44">
         <f t="shared" si="1"/>
@@ -1653,7 +1550,7 @@
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B46" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -1674,12 +1571,12 @@
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B50" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="51" spans="2:6" ht="17" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C51">
         <f t="shared" ref="C51:C54" si="2">$C$2*D51+$C$3*E51</f>
@@ -1697,7 +1594,7 @@
     </row>
     <row r="52" spans="2:6" ht="17" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C52">
         <f t="shared" si="2"/>
@@ -1715,7 +1612,7 @@
     </row>
     <row r="53" spans="2:6" ht="17" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C53">
         <f t="shared" si="2"/>
@@ -1731,7 +1628,7 @@
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C54">
         <f t="shared" si="2"/>
@@ -1770,11 +1667,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC5DF7A8-08FA-2145-BADA-18AB879783DA}">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1788,45 +1683,45 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="7"/>
       <c r="F1" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1843,7 +1738,7 @@
         <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1861,7 +1756,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1869,7 +1764,7 @@
         <v>7</v>
       </c>
       <c r="C12">
-        <f t="shared" ref="C12:C28" si="0">$C$2*D12+$C$3*E12</f>
+        <f t="shared" ref="C12:C21" si="0">$C$2*D12+$C$3*E12</f>
         <v>2</v>
       </c>
       <c r="D12" s="4">
@@ -1879,12 +1774,12 @@
         <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
@@ -1897,12 +1792,12 @@
         <v>1</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
@@ -1915,12 +1810,12 @@
         <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
@@ -1933,12 +1828,12 @@
         <v>2</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
@@ -1951,12 +1846,12 @@
         <v>1</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
@@ -1967,12 +1862,12 @@
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
@@ -1982,12 +1877,12 @@
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
@@ -2000,12 +1895,12 @@
         <v>4</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
@@ -2018,12 +1913,12 @@
         <v>1</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
@@ -2036,426 +1931,124 @@
         <v>1</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="C23" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24">
-        <f>$C$2*D24+$C$3*E24</f>
-        <v>12</v>
-      </c>
-      <c r="D24" s="4">
-        <v>6</v>
-      </c>
-      <c r="E24" s="4">
-        <v>6</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="B24" s="2"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="D25" s="4">
-        <v>24</v>
-      </c>
-      <c r="E25" s="4">
-        <v>24</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>26</v>
+      <c r="B25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="D26" s="4">
-        <v>12</v>
-      </c>
-      <c r="E26" s="4">
-        <v>12</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="E26" s="4"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="D27" s="4">
-        <v>3</v>
-      </c>
-      <c r="E27" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="D28" s="4">
-        <v>4</v>
-      </c>
-      <c r="E28" s="4">
-        <v>4</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B30" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31">
-        <f t="shared" ref="C31:C35" si="1">$C$2*D31+$C$3*E31</f>
-        <v>12</v>
-      </c>
-      <c r="D31" s="4">
-        <v>6</v>
-      </c>
-      <c r="E31" s="4">
-        <v>6</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>52</v>
+      <c r="B27" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="D32" s="4">
-        <v>1</v>
-      </c>
-      <c r="E32" s="4">
-        <v>1</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>57</v>
+      <c r="B32" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="C33">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="D33" s="4">
-        <v>1</v>
-      </c>
-      <c r="E33" s="4">
-        <v>1</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>57</v>
+        <f t="shared" ref="C33:C36" si="1">$C$2*D33+$C$3*E33</f>
+        <v>0</v>
+      </c>
+      <c r="E33" s="4"/>
+      <c r="F33" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C34">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="D34" s="4">
-        <v>1</v>
-      </c>
-      <c r="E34" s="4">
-        <v>1</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>57</v>
+        <v>0</v>
+      </c>
+      <c r="E34" s="4"/>
+      <c r="F34" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C35">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="D35" s="4">
-        <v>1</v>
-      </c>
-      <c r="E35" s="4">
-        <v>1</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>38</v>
+        <v>0</v>
+      </c>
+      <c r="E35" s="4"/>
+      <c r="F35" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="E36" s="4"/>
+      <c r="F36" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B37" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F37" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
-        <v>35</v>
-      </c>
-      <c r="C38">
-        <f t="shared" ref="C38:C43" si="2">$C$2*D38+$C$3*E38</f>
-        <v>2</v>
-      </c>
-      <c r="D38" s="4">
-        <v>1</v>
-      </c>
-      <c r="E38" s="4">
-        <v>1</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
-        <v>37</v>
-      </c>
-      <c r="C39">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="D39" s="4">
-        <v>1</v>
-      </c>
-      <c r="E39" s="4">
-        <v>1</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="D40" s="4">
-        <v>1</v>
-      </c>
-      <c r="E40" s="4">
-        <v>1</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
-        <v>32</v>
-      </c>
-      <c r="C41">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="D41" s="4">
-        <v>1</v>
-      </c>
-      <c r="E41" s="4">
-        <v>1</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
-        <v>29</v>
-      </c>
-      <c r="C42">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="D42" s="4">
-        <v>4</v>
-      </c>
-      <c r="E42" s="4">
-        <v>4</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
-        <v>31</v>
-      </c>
-      <c r="C43">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="D43" s="4">
-        <v>1</v>
-      </c>
-      <c r="E43" s="4">
-        <v>1</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B45" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B46" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B47" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B50" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B51" t="s">
-        <v>78</v>
-      </c>
-      <c r="C51">
-        <f t="shared" ref="C51:C54" si="3">$C$2*D51+$C$3*E51</f>
-        <v>0</v>
-      </c>
-      <c r="E51" s="4"/>
-      <c r="F51" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B52" t="s">
-        <v>79</v>
-      </c>
-      <c r="C52">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E52" s="4"/>
-      <c r="F52" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
-        <v>80</v>
-      </c>
-      <c r="C53">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E53" s="4"/>
-      <c r="F53" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B54" t="s">
-        <v>81</v>
-      </c>
-      <c r="C54">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E54" s="4"/>
-      <c r="F54" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B55" t="s">
-        <v>82</v>
+      <c r="B37" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F28" r:id="rId1" xr:uid="{B8652947-DCE1-8A43-8EC5-70D5E282DA42}"/>
-    <hyperlink ref="F24" r:id="rId2" xr:uid="{89DB73F8-E5B4-5747-B647-630D123A1947}"/>
-    <hyperlink ref="F25" r:id="rId3" xr:uid="{5ADD20DA-C729-1E40-9857-D601D00A824D}"/>
-    <hyperlink ref="F26" r:id="rId4" xr:uid="{6320D86F-7495-CE40-B4C5-A1AF5BAFCCB2}"/>
-    <hyperlink ref="F35" r:id="rId5" xr:uid="{F7737515-119F-4B4F-B458-F057B62E38F5}"/>
-    <hyperlink ref="F32" r:id="rId6" xr:uid="{472BC695-383E-3746-90AA-F3322B8D4A71}"/>
-    <hyperlink ref="F33" r:id="rId7" xr:uid="{6BBDA64E-8A8B-2645-BA65-440C54C86B9D}"/>
-    <hyperlink ref="F43" r:id="rId8" xr:uid="{B263E63A-9800-DC4B-92CD-0FD5D14F2ACB}"/>
-    <hyperlink ref="F42" r:id="rId9" xr:uid="{724CC3D0-73BF-CD43-865E-A347BB7BB14C}"/>
-    <hyperlink ref="F41" r:id="rId10" xr:uid="{42ECFFC1-109F-CC41-93A0-C2DE507F998E}"/>
-    <hyperlink ref="F38" r:id="rId11" xr:uid="{B59C96D6-FB81-F446-BB1B-1BFFEE168540}"/>
-    <hyperlink ref="F39" r:id="rId12" xr:uid="{DC25E6C6-FB14-0A43-B2F2-7DEDB09B8DE5}"/>
-    <hyperlink ref="F34" r:id="rId13" xr:uid="{7AC34CA2-FD87-3141-90BF-E0149B164C1E}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId14"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5f810545-bb7d-498e-98a6-3cc8175571c8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="8077f6fe-c9e5-4688-b004-da2992bb8cd8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2666,20 +2259,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5f810545-bb7d-498e-98a6-3cc8175571c8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="8077f6fe-c9e5-4688-b004-da2992bb8cd8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA44028-4133-420E-8665-60C989F4E89B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D196A880-6C6D-4D69-8998-929C3B39CF40}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="8077f6fe-c9e5-4688-b004-da2992bb8cd8"/>
+    <ds:schemaRef ds:uri="5f810545-bb7d-498e-98a6-3cc8175571c8"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2704,18 +2304,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D196A880-6C6D-4D69-8998-929C3B39CF40}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAA44028-4133-420E-8665-60C989F4E89B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="8077f6fe-c9e5-4688-b004-da2992bb8cd8"/>
-    <ds:schemaRef ds:uri="5f810545-bb7d-498e-98a6-3cc8175571c8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>